<commit_message>
formate between each fio script
</commit_message>
<xml_diff>
--- a/write_data.xlsx
+++ b/write_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Standard Device Config.</t>
   </si>
@@ -29,6 +29,72 @@
   </si>
   <si>
     <t>1.02 TB</t>
+  </si>
+  <si>
+    <t>BURST SEQUENTIAL WRITE</t>
+  </si>
+  <si>
+    <t>BURST SEQUENTIAL READ</t>
+  </si>
+  <si>
+    <t>BURST RANDOM WRITE</t>
+  </si>
+  <si>
+    <t>BURST RANDOM READ</t>
+  </si>
+  <si>
+    <t>BURST RANDOM WRITE OIO</t>
+  </si>
+  <si>
+    <t>BURST RANDOM READ OIO</t>
+  </si>
+  <si>
+    <t>SUBSTAIN SEQUENTIAL WRITE</t>
+  </si>
+  <si>
+    <t>BLOCK SIZE</t>
+  </si>
+  <si>
+    <t>IO-DEPTHS</t>
+  </si>
+  <si>
+    <t>THREADS</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>PRECONDITION</t>
+  </si>
+  <si>
+    <t>IOPS</t>
+  </si>
+  <si>
+    <t>BANDWIDTH</t>
+  </si>
+  <si>
+    <t>AVG, LATENCY</t>
+  </si>
+  <si>
+    <t>50th</t>
+  </si>
+  <si>
+    <t>75th</t>
+  </si>
+  <si>
+    <t>99th</t>
+  </si>
+  <si>
+    <t>99.9th</t>
+  </si>
+  <si>
+    <t>99.99th</t>
+  </si>
+  <si>
+    <t>99.999th</t>
+  </si>
+  <si>
+    <t>99.9999th</t>
   </si>
 </sst>
 </file>
@@ -360,18 +426,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -379,7 +445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -387,44 +453,91 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="5" spans="1:16">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>